<commit_message>
Complete WiFi bridge onboarding manual test for IOS 2.3.1 in #192
</commit_message>
<xml_diff>
--- a/App_Release/IOS/v2.3.1/Zeus_IOS_v2_3_1.xlsx
+++ b/App_Release/IOS/v2.3.1/Zeus_IOS_v2_3_1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\My Drive\001-Github\RYSE_Testing_record\App_Release\IOS\v2.3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947584AB-F16B-4CDD-AEDA-7338569345B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80E4FD1-C4C0-4B58-B172-5BB6D8DFD22E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{7785C230-C9C6-4B37-86E6-FED87339FA29}"/>
+    <workbookView xWindow="34425" yWindow="1980" windowWidth="21600" windowHeight="11235" activeTab="2" xr2:uid="{7785C230-C9C6-4B37-86E6-FED87339FA29}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary_v2" sheetId="2" r:id="rId1"/>
     <sheet name="Summary" sheetId="1" r:id="rId2"/>
+    <sheet name="BLE_Shade_test" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="267">
   <si>
     <t>Code</t>
   </si>
@@ -810,6 +811,66 @@
   </si>
   <si>
     <t>Date: 14-07-2025</t>
+  </si>
+  <si>
+    <t>15-07-2025</t>
+  </si>
+  <si>
+    <t>BLE Shade pair (focus update v3.10.0)</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time Start</t>
+  </si>
+  <si>
+    <t>Time End</t>
+  </si>
+  <si>
+    <t>UX</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Failed Connection during onbarding update -&gt; Back to update page</t>
+  </si>
+  <si>
+    <t>Failed to connect again x 3</t>
+  </si>
+  <si>
+    <t>Failed to connect again x 5</t>
+  </si>
+  <si>
+    <t>Enter shade control page and focus update -&gt; Fail</t>
+  </si>
+  <si>
+    <t>Focus update during onboarding</t>
+  </si>
+  <si>
+    <t>Remark &amp; Issue</t>
+  </si>
+  <si>
+    <t>Success in fifth attempt</t>
+  </si>
+  <si>
+    <t>Failed to connect again x 2</t>
+  </si>
+  <si>
+    <t>Success in second attempt</t>
+  </si>
+  <si>
+    <t>Success in third attempt</t>
+  </si>
+  <si>
+    <t>Enter shade control page and focus update x4 -&gt; Pass</t>
+  </si>
+  <si>
+    <t>Enter shade control page and focus update x5 -&gt; Pass</t>
   </si>
 </sst>
 </file>
@@ -871,7 +932,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -929,6 +990,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1041,7 +1120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1070,37 +1149,36 @@
     <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1110,14 +1188,40 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="39">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5D5D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1405,6 +1509,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF5D5D"/>
       <color rgb="FF9EDCF0"/>
       <color rgb="FFAED4F4"/>
       <color rgb="FFB1E0FD"/>
@@ -1414,7 +1519,6 @@
       <color rgb="FFDFCBF5"/>
       <color rgb="FFFBCDED"/>
       <color rgb="FFFDE3F5"/>
-      <color rgb="FFF5B9DB"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1747,8 +1851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{970B1C3B-E1AB-41A9-8F2A-32BDA9DC678F}">
   <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1761,13 +1865,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
       <c r="F1" s="17" t="s">
         <v>246</v>
       </c>
@@ -2516,7 +2620,7 @@
       <c r="E44" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="F44" s="34" t="s">
+      <c r="F44" s="28" t="s">
         <v>242</v>
       </c>
     </row>
@@ -3178,101 +3282,98 @@
       <c r="F86" s="7"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="33" t="s">
+      <c r="A88" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="B88" s="33"/>
-      <c r="C88" s="33"/>
-      <c r="D88" s="33"/>
-      <c r="E88" s="33"/>
-      <c r="F88" s="33"/>
+      <c r="B88" s="36"/>
+      <c r="C88" s="36"/>
+      <c r="D88" s="36"/>
+      <c r="E88" s="36"/>
+      <c r="F88" s="36"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B89" s="30" t="s">
+      <c r="B89" s="39" t="s">
         <v>244</v>
       </c>
-      <c r="C89" s="30"/>
-      <c r="D89" s="30"/>
-      <c r="E89" s="30"/>
-      <c r="F89" s="30"/>
+      <c r="C89" s="39"/>
+      <c r="D89" s="39"/>
+      <c r="E89" s="39"/>
+      <c r="F89" s="39"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B90" s="35" t="s">
+      <c r="B90" s="40" t="s">
         <v>245</v>
       </c>
-      <c r="C90" s="35"/>
-      <c r="D90" s="35"/>
-      <c r="E90" s="35"/>
-      <c r="F90" s="35"/>
+      <c r="C90" s="40"/>
+      <c r="D90" s="40"/>
+      <c r="E90" s="40"/>
+      <c r="F90" s="40"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B91" s="30" t="s">
+      <c r="B91" s="39" t="s">
         <v>222</v>
       </c>
-      <c r="C91" s="30"/>
-      <c r="D91" s="30"/>
-      <c r="E91" s="30"/>
-      <c r="F91" s="30"/>
+      <c r="C91" s="39"/>
+      <c r="D91" s="39"/>
+      <c r="E91" s="39"/>
+      <c r="F91" s="39"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B92" s="30" t="s">
+      <c r="B92" s="39" t="s">
         <v>233</v>
       </c>
-      <c r="C92" s="30"/>
-      <c r="D92" s="30"/>
-      <c r="E92" s="30"/>
-      <c r="F92" s="30"/>
+      <c r="C92" s="39"/>
+      <c r="D92" s="39"/>
+      <c r="E92" s="39"/>
+      <c r="F92" s="39"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B93" s="41" t="s">
+      <c r="B93" s="42" t="s">
         <v>234</v>
       </c>
-      <c r="C93" s="42"/>
-      <c r="D93" s="42"/>
-      <c r="E93" s="42"/>
-      <c r="F93" s="43"/>
+      <c r="C93" s="43"/>
+      <c r="D93" s="43"/>
+      <c r="E93" s="43"/>
+      <c r="F93" s="44"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A94" s="39" t="s">
+      <c r="A94" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B94" s="36" t="s">
+      <c r="B94" s="41" t="s">
         <v>227</v>
       </c>
-      <c r="C94" s="36"/>
-      <c r="D94" s="36"/>
-      <c r="E94" s="36"/>
-      <c r="F94" s="36"/>
+      <c r="C94" s="41"/>
+      <c r="D94" s="41"/>
+      <c r="E94" s="41"/>
+      <c r="F94" s="41"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A95" s="38" t="s">
+      <c r="A95" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="B95" s="44" t="s">
+      <c r="B95" s="37" t="s">
         <v>237</v>
       </c>
-      <c r="C95" s="37"/>
-      <c r="D95" s="37"/>
-      <c r="E95" s="37"/>
-      <c r="F95" s="37"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" s="40"/>
+      <c r="C95" s="38"/>
+      <c r="D95" s="38"/>
+      <c r="E95" s="38"/>
+      <c r="F95" s="38"/>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
@@ -3291,6 +3392,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A88:F88"/>
     <mergeCell ref="B95:F95"/>
     <mergeCell ref="B89:F89"/>
     <mergeCell ref="B90:F90"/>
@@ -3298,50 +3401,48 @@
     <mergeCell ref="B92:F92"/>
     <mergeCell ref="B94:F94"/>
     <mergeCell ref="B93:F93"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A88:F88"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="36" priority="5" operator="containsText" text="BX1">
+    <cfRule type="containsText" dxfId="38" priority="5" operator="containsText" text="BX1">
       <formula>NOT(ISERROR(SEARCH("BX1",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="8" operator="containsText" text="CB0">
+    <cfRule type="containsText" dxfId="37" priority="8" operator="containsText" text="CB0">
       <formula>NOT(ISERROR(SEARCH("CB0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="9" operator="containsText" text="CR0">
+    <cfRule type="containsText" dxfId="36" priority="9" operator="containsText" text="CR0">
       <formula>NOT(ISERROR(SEARCH("CR0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="10" operator="containsText" text="CG0">
+    <cfRule type="containsText" dxfId="35" priority="10" operator="containsText" text="CG0">
       <formula>NOT(ISERROR(SEARCH("CG0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="11" operator="containsText" text="CX0">
+    <cfRule type="containsText" dxfId="34" priority="11" operator="containsText" text="CX0">
       <formula>NOT(ISERROR(SEARCH("CX0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="12" operator="containsText" text="MX0">
+    <cfRule type="containsText" dxfId="33" priority="12" operator="containsText" text="MX0">
       <formula>NOT(ISERROR(SEARCH("MX0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="13" operator="containsText" text="OT0">
+    <cfRule type="containsText" dxfId="32" priority="13" operator="containsText" text="OT0">
       <formula>NOT(ISERROR(SEARCH("OT0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="14" operator="containsText" text="CS0">
+    <cfRule type="containsText" dxfId="31" priority="14" operator="containsText" text="CS0">
       <formula>NOT(ISERROR(SEARCH("CS0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="15" operator="containsText" text="RX0">
+    <cfRule type="containsText" dxfId="30" priority="15" operator="containsText" text="RX0">
       <formula>NOT(ISERROR(SEARCH("RX0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="16" operator="containsText" text="GX0">
+    <cfRule type="containsText" dxfId="29" priority="16" operator="containsText" text="GX0">
       <formula>NOT(ISERROR(SEARCH("GX0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="17" operator="containsText" text="SB0">
+    <cfRule type="containsText" dxfId="28" priority="17" operator="containsText" text="SB0">
       <formula>NOT(ISERROR(SEARCH("SB0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="18" operator="containsText" text="SX0">
+    <cfRule type="containsText" dxfId="27" priority="18" operator="containsText" text="SX0">
       <formula>NOT(ISERROR(SEARCH("SX0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="19" operator="containsText" text="BX0">
+    <cfRule type="containsText" dxfId="26" priority="19" operator="containsText" text="BX0">
       <formula>NOT(ISERROR(SEARCH("BX0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="20" operator="containsText" text="AX0">
+    <cfRule type="containsText" dxfId="25" priority="20" operator="containsText" text="AX0">
       <formula>NOT(ISERROR(SEARCH("AX0",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3374,28 +3475,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D87">
-    <cfRule type="containsText" dxfId="22" priority="1" operator="containsText" text="Fixed">
+    <cfRule type="containsText" dxfId="24" priority="1" operator="containsText" text="Fixed">
       <formula>NOT(ISERROR(SEARCH("Fixed",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D87">
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D96">
-    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D96:D1048576">
-    <cfRule type="containsText" dxfId="17" priority="6" operator="containsText" text="Fixed">
+    <cfRule type="containsText" dxfId="19" priority="6" operator="containsText" text="Fixed">
       <formula>NOT(ISERROR(SEARCH("Fixed",D96)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3453,13 +3554,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
       <c r="F1" s="17" t="s">
         <v>169</v>
       </c>
@@ -4659,49 +4760,49 @@
       <c r="F86" s="7"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B88" s="33" t="s">
+      <c r="B88" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="C88" s="33"/>
-      <c r="D88" s="33"/>
-      <c r="E88" s="33"/>
+      <c r="C88" s="36"/>
+      <c r="D88" s="36"/>
+      <c r="E88" s="36"/>
       <c r="F88" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B89" s="30" t="s">
+      <c r="B89" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="C89" s="30"/>
-      <c r="D89" s="30"/>
-      <c r="E89" s="30"/>
+      <c r="C89" s="39"/>
+      <c r="D89" s="39"/>
+      <c r="E89" s="39"/>
       <c r="F89" s="22" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B90" s="31" t="s">
+      <c r="B90" s="46" t="s">
         <v>173</v>
       </c>
-      <c r="C90" s="31"/>
-      <c r="D90" s="31"/>
-      <c r="E90" s="31"/>
+      <c r="C90" s="46"/>
+      <c r="D90" s="46"/>
+      <c r="E90" s="46"/>
       <c r="F90" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B91" s="32"/>
-      <c r="C91" s="32"/>
-      <c r="D91" s="32"/>
-      <c r="E91" s="32"/>
+      <c r="B91" s="47"/>
+      <c r="C91" s="47"/>
+      <c r="D91" s="47"/>
+      <c r="E91" s="47"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B92" s="28"/>
-      <c r="C92" s="28"/>
-      <c r="D92" s="28"/>
-      <c r="E92" s="28"/>
+      <c r="B92" s="45"/>
+      <c r="C92" s="45"/>
+      <c r="D92" s="45"/>
+      <c r="E92" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4714,46 +4815,46 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="BX1">
+    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="BX1">
       <formula>NOT(ISERROR(SEARCH("BX1",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="CB0">
+    <cfRule type="containsText" dxfId="17" priority="6" operator="containsText" text="CB0">
       <formula>NOT(ISERROR(SEARCH("CB0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="7" operator="containsText" text="CR0">
+    <cfRule type="containsText" dxfId="16" priority="7" operator="containsText" text="CR0">
       <formula>NOT(ISERROR(SEARCH("CR0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="CG0">
+    <cfRule type="containsText" dxfId="15" priority="8" operator="containsText" text="CG0">
       <formula>NOT(ISERROR(SEARCH("CG0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="CX0">
+    <cfRule type="containsText" dxfId="14" priority="9" operator="containsText" text="CX0">
       <formula>NOT(ISERROR(SEARCH("CX0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="MX0">
+    <cfRule type="containsText" dxfId="13" priority="10" operator="containsText" text="MX0">
       <formula>NOT(ISERROR(SEARCH("MX0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="OT0">
+    <cfRule type="containsText" dxfId="12" priority="11" operator="containsText" text="OT0">
       <formula>NOT(ISERROR(SEARCH("OT0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="CS0">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="CS0">
       <formula>NOT(ISERROR(SEARCH("CS0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="13" operator="containsText" text="RX0">
+    <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="RX0">
       <formula>NOT(ISERROR(SEARCH("RX0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="14" operator="containsText" text="GX0">
+    <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="GX0">
       <formula>NOT(ISERROR(SEARCH("GX0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="15" operator="containsText" text="SB0">
+    <cfRule type="containsText" dxfId="8" priority="15" operator="containsText" text="SB0">
       <formula>NOT(ISERROR(SEARCH("SB0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="16" operator="containsText" text="SX0">
+    <cfRule type="containsText" dxfId="7" priority="16" operator="containsText" text="SX0">
       <formula>NOT(ISERROR(SEARCH("SX0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="17" operator="containsText" text="BX0">
+    <cfRule type="containsText" dxfId="6" priority="17" operator="containsText" text="BX0">
       <formula>NOT(ISERROR(SEARCH("BX0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="18" operator="containsText" text="AX0">
+    <cfRule type="containsText" dxfId="5" priority="18" operator="containsText" text="AX0">
       <formula>NOT(ISERROR(SEARCH("AX0",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4772,15 +4873,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D91 D93:D1048576">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Fixed">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Fixed">
       <formula>NOT(ISERROR(SEARCH("Fixed",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D87 D93:D95">
-    <cfRule type="cellIs" dxfId="1" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="19" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="20" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4806,4 +4907,383 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47CF2177-A47C-4907-A8C0-D76F9C54A8AB}">
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="59.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="47.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="48" t="s">
+        <v>248</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="31" t="s">
+        <v>249</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>252</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>253</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="G2" s="49" t="s">
+        <v>260</v>
+      </c>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>247</v>
+      </c>
+      <c r="C3" s="33">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="D3" s="33">
+        <v>0.62361111111111112</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C4" s="33">
+        <v>0.625</v>
+      </c>
+      <c r="D4" s="33">
+        <v>0.62777777777777777</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>247</v>
+      </c>
+      <c r="C5" s="33">
+        <v>0.62916666666666665</v>
+      </c>
+      <c r="D5" s="33">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C6" s="33">
+        <v>0.63263888888888886</v>
+      </c>
+      <c r="D6" s="33">
+        <v>0.63749999999999996</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>247</v>
+      </c>
+      <c r="C7" s="33">
+        <v>0.6381944444444444</v>
+      </c>
+      <c r="D7" s="33">
+        <v>0.64097222222222228</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C8" s="33">
+        <v>0.64513888888888893</v>
+      </c>
+      <c r="D8" s="33">
+        <v>0.6479166666666667</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>247</v>
+      </c>
+      <c r="C9" s="33">
+        <v>0.64861111111111114</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0.65347222222222223</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C10" s="33">
+        <v>0.65416666666666667</v>
+      </c>
+      <c r="D10" s="33">
+        <v>0.65694444444444444</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="J10" s="34" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>247</v>
+      </c>
+      <c r="C11" s="33">
+        <v>0.65833333333333333</v>
+      </c>
+      <c r="D11" s="33">
+        <v>0.66111111111111109</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="J11" s="34" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C12" s="33">
+        <v>0.66111111111111109</v>
+      </c>
+      <c r="D12" s="33">
+        <v>0.66319444444444442</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="J12" s="34" t="s">
+        <v>265</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="G2:J2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>